<commit_message>
removed try exception statement in app.py
</commit_message>
<xml_diff>
--- a/ps.xlsx
+++ b/ps.xlsx
@@ -446,1313 +446,1313 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2775V</t>
+          <t>9123C</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>85.09999999999999</v>
+        <v>86.8</v>
       </c>
       <c r="C2" t="n">
-        <v>83.59999999999999</v>
+        <v>87.5</v>
       </c>
       <c r="D2" t="n">
-        <v>84.09999999999999</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>9364H</t>
+          <t>8110V</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>81</v>
+        <v>80.2</v>
       </c>
       <c r="C3" t="n">
-        <v>86.3</v>
+        <v>78.5</v>
       </c>
       <c r="D3" t="n">
-        <v>83.2</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>13358C</t>
+          <t>323V</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>79.59999999999999</v>
+        <v>79.7</v>
       </c>
       <c r="C4" t="n">
-        <v>83.09999999999999</v>
+        <v>78.2</v>
       </c>
       <c r="D4" t="n">
-        <v>80.90000000000001</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7925X</t>
+          <t>117B</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>78.8</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>79.8</v>
+        <v>76.2</v>
       </c>
       <c r="D5" t="n">
-        <v>78.59999999999999</v>
+        <v>79.59999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>99904X</t>
+          <t>70291D</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>75.7</v>
+        <v>77.3</v>
       </c>
       <c r="C6" t="n">
-        <v>54.7</v>
+        <v>69.5</v>
       </c>
       <c r="D6" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>50252A</t>
+          <t>2654P</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>74.59999999999999</v>
+        <v>77.3</v>
       </c>
       <c r="C7" t="n">
-        <v>75.2</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>72.3</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>8829C</t>
+          <t>1010W</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>72.5</v>
+        <v>77.2</v>
       </c>
       <c r="C8" t="n">
-        <v>69.3</v>
+        <v>80.3</v>
       </c>
       <c r="D8" t="n">
-        <v>69.59999999999999</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>78792E</t>
+          <t>1064B</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>70.3</v>
+        <v>73.3</v>
       </c>
       <c r="C9" t="n">
-        <v>61.7</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>67.59999999999999</v>
+        <v>69.40000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>67101G</t>
+          <t>3135B</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>68.8</v>
+        <v>72.8</v>
       </c>
       <c r="C10" t="n">
-        <v>59.3</v>
+        <v>70.90000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>63.6</v>
+        <v>69.8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1229W</t>
+          <t>55286A</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>68.7</v>
+        <v>72.7</v>
       </c>
       <c r="C11" t="n">
-        <v>59.6</v>
+        <v>80.2</v>
       </c>
       <c r="D11" t="n">
-        <v>66.5</v>
+        <v>73.09999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2131Y</t>
+          <t>4082B</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>68.5</v>
+        <v>72.5</v>
       </c>
       <c r="C12" t="n">
-        <v>68.7</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>60.7</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>8076X</t>
+          <t>2496J</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>67.7</v>
+        <v>69.2</v>
       </c>
       <c r="C13" t="n">
-        <v>67.8</v>
+        <v>72</v>
       </c>
       <c r="D13" t="n">
-        <v>66.7</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>7316X</t>
+          <t>5155E</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>66.2</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>75.3</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="D14" t="n">
-        <v>62.5</v>
+        <v>56.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>210T</t>
+          <t>2011F</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>65.8</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>69.5</v>
+        <v>75.8</v>
       </c>
       <c r="D15" t="n">
-        <v>69.2</v>
+        <v>69.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>82855S</t>
+          <t>871X</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>64.8</v>
+        <v>67.7</v>
       </c>
       <c r="C16" t="n">
-        <v>72.09999999999999</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="D16" t="n">
-        <v>60.9</v>
+        <v>71.90000000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20096G</t>
+          <t>51581E</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>63.4</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="C17" t="n">
-        <v>67.90000000000001</v>
+        <v>65.2</v>
       </c>
       <c r="D17" t="n">
-        <v>73</v>
+        <v>62.3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2055A</t>
+          <t>39313Z</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>62.9</v>
+        <v>67.3</v>
       </c>
       <c r="C18" t="n">
-        <v>60.3</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>61.6</v>
+        <v>67.40000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>9039N</t>
+          <t>12X</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>62.8</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>56.6</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>63.6</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3796H</t>
+          <t>15442C</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>61.4</v>
+        <v>65.2</v>
       </c>
       <c r="C20" t="n">
-        <v>58.7</v>
+        <v>59.4</v>
       </c>
       <c r="D20" t="n">
-        <v>63.7</v>
+        <v>63.9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>9909Y</t>
+          <t>96504E</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>60.6</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="C21" t="n">
-        <v>63.3</v>
+        <v>60.5</v>
       </c>
       <c r="D21" t="n">
-        <v>67.3</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1898A</t>
+          <t>62880A</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>60.1</v>
+        <v>64.2</v>
       </c>
       <c r="C22" t="n">
-        <v>60.9</v>
+        <v>66.2</v>
       </c>
       <c r="D22" t="n">
-        <v>55.4</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>61002G</t>
+          <t>1669X</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>59.9</v>
+        <v>60.4</v>
       </c>
       <c r="C23" t="n">
-        <v>67.40000000000001</v>
+        <v>58</v>
       </c>
       <c r="D23" t="n">
-        <v>59.2</v>
+        <v>62.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3145H</t>
+          <t>74947K</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>59.9</v>
+        <v>60</v>
       </c>
       <c r="C24" t="n">
-        <v>56.1</v>
+        <v>64.5</v>
       </c>
       <c r="D24" t="n">
-        <v>61.1</v>
+        <v>58.7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1727N</t>
+          <t>7110H</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>59.9</v>
+        <v>58.9</v>
       </c>
       <c r="C25" t="n">
-        <v>52.9</v>
+        <v>60.1</v>
       </c>
       <c r="D25" t="n">
-        <v>58.6</v>
+        <v>61.4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>7187K</t>
+          <t>355U</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>59.2</v>
+        <v>58.6</v>
       </c>
       <c r="C26" t="n">
-        <v>47.9</v>
+        <v>57</v>
       </c>
       <c r="D26" t="n">
-        <v>56</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>987X</t>
+          <t>17022A</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" t="n">
-        <v>51</v>
+        <v>58.1</v>
       </c>
       <c r="D27" t="n">
-        <v>56.5</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>315E</t>
+          <t>20541B</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>58.6</v>
+        <v>56.9</v>
       </c>
       <c r="C28" t="n">
-        <v>61.5</v>
+        <v>59.7</v>
       </c>
       <c r="D28" t="n">
-        <v>61.5</v>
+        <v>55.9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>338A</t>
+          <t>10478K</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>58.5</v>
+        <v>55.4</v>
       </c>
       <c r="C29" t="n">
-        <v>65.59999999999999</v>
+        <v>62.2</v>
       </c>
       <c r="D29" t="n">
-        <v>59</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1394A</t>
+          <t>7996D</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>58.4</v>
+        <v>54.9</v>
       </c>
       <c r="C30" t="n">
-        <v>54.4</v>
+        <v>58</v>
       </c>
       <c r="D30" t="n">
-        <v>62.1</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>729S</t>
+          <t>6627S</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>57.9</v>
+        <v>54.8</v>
       </c>
       <c r="C31" t="n">
-        <v>61.1</v>
+        <v>52.8</v>
       </c>
       <c r="D31" t="n">
-        <v>54.1</v>
+        <v>48.9</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>393C</t>
+          <t>2105A</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>57.3</v>
+        <v>54.8</v>
       </c>
       <c r="C32" t="n">
-        <v>55</v>
+        <v>62.6</v>
       </c>
       <c r="D32" t="n">
-        <v>55.5</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>11124P</t>
+          <t>1158X</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>56.9</v>
+        <v>53.4</v>
       </c>
       <c r="C33" t="n">
-        <v>60</v>
+        <v>49.4</v>
       </c>
       <c r="D33" t="n">
-        <v>51.2</v>
+        <v>55.2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>74177H</t>
+          <t>295R</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>56.8</v>
+        <v>52.9</v>
       </c>
       <c r="C34" t="n">
-        <v>45.1</v>
+        <v>43.4</v>
       </c>
       <c r="D34" t="n">
-        <v>53.9</v>
+        <v>48.9</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4583X</t>
+          <t>4886W</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>55.9</v>
+        <v>52.3</v>
       </c>
       <c r="C35" t="n">
-        <v>50.5</v>
+        <v>45</v>
       </c>
       <c r="D35" t="n">
-        <v>51</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>75503Z</t>
+          <t>32174C</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>54.2</v>
+        <v>52.2</v>
       </c>
       <c r="C36" t="n">
-        <v>67.09999999999999</v>
+        <v>59.9</v>
       </c>
       <c r="D36" t="n">
-        <v>55.8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>98548D</t>
+          <t>8787A</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>52.8</v>
+        <v>52</v>
       </c>
       <c r="C37" t="n">
-        <v>51.1</v>
+        <v>51.7</v>
       </c>
       <c r="D37" t="n">
-        <v>56.5</v>
+        <v>48.6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>33418X</t>
+          <t>1353M</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>52.6</v>
+        <v>51.4</v>
       </c>
       <c r="C38" t="n">
-        <v>62.6</v>
+        <v>61.1</v>
       </c>
       <c r="D38" t="n">
-        <v>55.2</v>
+        <v>55.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5069R</t>
+          <t>89227A</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>52.5</v>
+        <v>50.7</v>
       </c>
       <c r="C39" t="n">
-        <v>58.8</v>
+        <v>34.1</v>
       </c>
       <c r="D39" t="n">
-        <v>54</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2550R</t>
+          <t>71909Z</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="C40" t="n">
-        <v>55.2</v>
+        <v>40.7</v>
       </c>
       <c r="D40" t="n">
-        <v>52.1</v>
+        <v>43.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>10N</t>
+          <t>77275B</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>52.2</v>
+        <v>49.9</v>
       </c>
       <c r="C41" t="n">
-        <v>47.5</v>
+        <v>57.2</v>
       </c>
       <c r="D41" t="n">
-        <v>50.9</v>
+        <v>51.2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4154V</t>
+          <t>945C</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>52.1</v>
+        <v>49.8</v>
       </c>
       <c r="C42" t="n">
-        <v>50.3</v>
+        <v>61.3</v>
       </c>
       <c r="D42" t="n">
-        <v>46.2</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1028Z</t>
+          <t>34690A</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>49.9</v>
+        <v>49.5</v>
       </c>
       <c r="C43" t="n">
-        <v>49.4</v>
+        <v>42.3</v>
       </c>
       <c r="D43" t="n">
-        <v>49.2</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>53171E</t>
+          <t>99751F</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>49.9</v>
+        <v>49.4</v>
       </c>
       <c r="C44" t="n">
-        <v>53.3</v>
+        <v>28.5</v>
       </c>
       <c r="D44" t="n">
-        <v>44.5</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>9181F</t>
+          <t>13974A</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>49.5</v>
+        <v>49</v>
       </c>
       <c r="C45" t="n">
-        <v>50.2</v>
+        <v>36.8</v>
       </c>
       <c r="D45" t="n">
-        <v>50.4</v>
+        <v>37.9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>44252N</t>
+          <t>64040C</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>49</v>
       </c>
       <c r="C46" t="n">
-        <v>52.5</v>
+        <v>59.6</v>
       </c>
       <c r="D46" t="n">
-        <v>51.7</v>
+        <v>46.7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>95569C</t>
+          <t>3457C</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>48.2</v>
+        <v>48.9</v>
       </c>
       <c r="C47" t="n">
-        <v>41.8</v>
+        <v>45.7</v>
       </c>
       <c r="D47" t="n">
-        <v>46.7</v>
+        <v>51.1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>80550F</t>
+          <t>56H</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>47.9</v>
+        <v>48.4</v>
       </c>
       <c r="C48" t="n">
-        <v>59.8</v>
+        <v>51</v>
       </c>
       <c r="D48" t="n">
-        <v>48.5</v>
+        <v>46.4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>91U</t>
+          <t>11495E</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>47.7</v>
+        <v>47.9</v>
       </c>
       <c r="C49" t="n">
-        <v>42.6</v>
+        <v>40.3</v>
       </c>
       <c r="D49" t="n">
-        <v>47.9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>654V</t>
+          <t>7882B</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>47.5</v>
+        <v>43.7</v>
       </c>
       <c r="C50" t="n">
-        <v>31.1</v>
+        <v>41.9</v>
       </c>
       <c r="D50" t="n">
-        <v>40.6</v>
+        <v>47.6</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>7842P</t>
+          <t>94517X</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>46.8</v>
+        <v>43.2</v>
       </c>
       <c r="C51" t="n">
-        <v>54.8</v>
+        <v>49.8</v>
       </c>
       <c r="D51" t="n">
-        <v>49.9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>57249C</t>
+          <t>59200X</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>46.5</v>
+        <v>43.2</v>
       </c>
       <c r="C52" t="n">
-        <v>52.2</v>
+        <v>37.1</v>
       </c>
       <c r="D52" t="n">
-        <v>46.9</v>
+        <v>38.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6844B</t>
+          <t>24842T</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>45.7</v>
+        <v>42.8</v>
       </c>
       <c r="C53" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D53" t="n">
-        <v>45.5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>39Z</t>
+          <t>81218C</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>45.6</v>
+        <v>42.4</v>
       </c>
       <c r="C54" t="n">
-        <v>52.6</v>
+        <v>57.6</v>
       </c>
       <c r="D54" t="n">
-        <v>49.6</v>
+        <v>46.6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>16329C</t>
+          <t>77353N</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>45.4</v>
+        <v>41.5</v>
       </c>
       <c r="C55" t="n">
-        <v>42.6</v>
+        <v>39.9</v>
       </c>
       <c r="D55" t="n">
-        <v>44.9</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>63310A</t>
+          <t>242W</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>45.4</v>
+        <v>41.5</v>
       </c>
       <c r="C56" t="n">
-        <v>56.2</v>
+        <v>22.4</v>
       </c>
       <c r="D56" t="n">
-        <v>48.8</v>
+        <v>35.8</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5430A</t>
+          <t>84260C</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>44.6</v>
+        <v>41.2</v>
       </c>
       <c r="C57" t="n">
-        <v>42.7</v>
+        <v>33.4</v>
       </c>
       <c r="D57" t="n">
-        <v>41.6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>36867D</t>
+          <t>603B</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>44.1</v>
+        <v>41</v>
       </c>
       <c r="C58" t="n">
-        <v>51.5</v>
+        <v>52.5</v>
       </c>
       <c r="D58" t="n">
-        <v>40.5</v>
+        <v>39.7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2335D</t>
+          <t>7282K</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>43.5</v>
+        <v>40.8</v>
       </c>
       <c r="C59" t="n">
-        <v>56.3</v>
+        <v>40.9</v>
       </c>
       <c r="D59" t="n">
-        <v>56</v>
+        <v>43.6</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>255M</t>
+          <t>502X</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>42.5</v>
+        <v>40.7</v>
       </c>
       <c r="C60" t="n">
-        <v>46.4</v>
+        <v>43.2</v>
       </c>
       <c r="D60" t="n">
-        <v>42.6</v>
+        <v>38.7</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6219A</t>
+          <t>7580Z</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>42.4</v>
+        <v>40.4</v>
       </c>
       <c r="C61" t="n">
-        <v>44.6</v>
+        <v>34.9</v>
       </c>
       <c r="D61" t="n">
-        <v>39.9</v>
+        <v>44.8</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>66086J</t>
+          <t>97834C</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>42.3</v>
+        <v>40</v>
       </c>
       <c r="C62" t="n">
-        <v>46.8</v>
+        <v>52.1</v>
       </c>
       <c r="D62" t="n">
-        <v>47.5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>3723X</t>
+          <t>2158Z</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>42.2</v>
+        <v>38.4</v>
       </c>
       <c r="C63" t="n">
-        <v>37.8</v>
+        <v>47.4</v>
       </c>
       <c r="D63" t="n">
-        <v>42.8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>8568A</t>
+          <t>9328Z</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>38.3</v>
+        <v>37.6</v>
       </c>
       <c r="C64" t="n">
-        <v>34.1</v>
+        <v>37.4</v>
       </c>
       <c r="D64" t="n">
-        <v>30.3</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>14904B</t>
+          <t>2915X</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>37</v>
+        <v>34.6</v>
       </c>
       <c r="C65" t="n">
-        <v>37.2</v>
+        <v>29.6</v>
       </c>
       <c r="D65" t="n">
-        <v>39.8</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>3350C</t>
+          <t>9727A</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>36.9</v>
+        <v>34.6</v>
       </c>
       <c r="C66" t="n">
-        <v>33.9</v>
+        <v>32.1</v>
       </c>
       <c r="D66" t="n">
-        <v>39</v>
+        <v>35.2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3017X</t>
+          <t>1764X</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>36.6</v>
+        <v>34.4</v>
       </c>
       <c r="C67" t="n">
-        <v>46.1</v>
+        <v>27.2</v>
       </c>
       <c r="D67" t="n">
-        <v>41</v>
+        <v>34.3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>550C</t>
+          <t>29760E</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>35.6</v>
+        <v>34.3</v>
       </c>
       <c r="C68" t="n">
-        <v>39.3</v>
+        <v>44.5</v>
       </c>
       <c r="D68" t="n">
-        <v>31.3</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>1082S</t>
+          <t>6104G</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>33.8</v>
+        <v>32.7</v>
       </c>
       <c r="C69" t="n">
-        <v>29.1</v>
+        <v>32.3</v>
       </c>
       <c r="D69" t="n">
-        <v>29.7</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>42368B</t>
+          <t>4405W</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>33.3</v>
+        <v>32.7</v>
       </c>
       <c r="C70" t="n">
-        <v>46.4</v>
+        <v>25.9</v>
       </c>
       <c r="D70" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>5956D</t>
+          <t>18687A</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>32.5</v>
+        <v>32.6</v>
       </c>
       <c r="C71" t="n">
-        <v>34</v>
+        <v>40.2</v>
       </c>
       <c r="D71" t="n">
-        <v>29.5</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>97027E</t>
+          <t>5735H</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>28.7</v>
+        <v>32.4</v>
       </c>
       <c r="C72" t="n">
-        <v>27.9</v>
+        <v>34.4</v>
       </c>
       <c r="D72" t="n">
-        <v>27.5</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>70761S</t>
+          <t>19800A</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>27.7</v>
+        <v>30.7</v>
       </c>
       <c r="C73" t="n">
-        <v>41.8</v>
+        <v>42</v>
       </c>
       <c r="D73" t="n">
-        <v>35.4</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>99153Z</t>
+          <t>8892A</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>27.7</v>
+        <v>30.3</v>
       </c>
       <c r="C74" t="n">
-        <v>24.6</v>
+        <v>40.5</v>
       </c>
       <c r="D74" t="n">
-        <v>33</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>21444J</t>
+          <t>45250J</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>26.6</v>
+        <v>30.2</v>
       </c>
       <c r="C75" t="n">
-        <v>13</v>
+        <v>39.9</v>
       </c>
       <c r="D75" t="n">
-        <v>29.3</v>
+        <v>35.8</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>88019A</t>
+          <t>675D</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>24.9</v>
+        <v>29.2</v>
       </c>
       <c r="C76" t="n">
-        <v>30.7</v>
+        <v>34.1</v>
       </c>
       <c r="D76" t="n">
-        <v>24.6</v>
+        <v>31.4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>30410V</t>
+          <t>43146C</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>24.7</v>
+        <v>29.1</v>
       </c>
       <c r="C77" t="n">
-        <v>22.5</v>
+        <v>22</v>
       </c>
       <c r="D77" t="n">
-        <v>25.8</v>
+        <v>31.3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>93303X</t>
+          <t>79267V</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>24.1</v>
+        <v>25.3</v>
       </c>
       <c r="C78" t="n">
-        <v>24.2</v>
+        <v>29.4</v>
       </c>
       <c r="D78" t="n">
-        <v>20.2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>17760X</t>
+          <t>48321H</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>23.4</v>
+        <v>22.8</v>
       </c>
       <c r="C79" t="n">
-        <v>18.7</v>
+        <v>17.2</v>
       </c>
       <c r="D79" t="n">
-        <v>23.3</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>46692A</t>
+          <t>3249V</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>22.6</v>
+        <v>21.3</v>
       </c>
       <c r="C80" t="n">
-        <v>18.3</v>
+        <v>19.2</v>
       </c>
       <c r="D80" t="n">
-        <v>24.6</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>27508D</t>
+          <t>3773W</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>20.3</v>
+        <v>18.8</v>
       </c>
       <c r="C81" t="n">
-        <v>21.4</v>
+        <v>26.6</v>
       </c>
       <c r="D81" t="n">
-        <v>20.7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>901Z</t>
+          <t>99040S</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>15.8</v>
+        <v>18.4</v>
       </c>
       <c r="C82" t="n">
-        <v>14.4</v>
+        <v>20</v>
       </c>
       <c r="D82" t="n">
-        <v>17</v>
+        <v>13.6</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>18908X</t>
+          <t>66800K</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>8.800000000000001</v>
+        <v>9</v>
       </c>
       <c r="C83" t="n">
-        <v>5.8</v>
+        <v>7.9</v>
       </c>
       <c r="D83" t="n">
-        <v>10.4</v>
+        <v>7.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>